<commit_message>
Oanda File new try
</commit_message>
<xml_diff>
--- a/archivos/archivo_tradeview_1.xlsx
+++ b/archivos/archivo_tradeview_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/84f1aedc942e402d/Documentos/GitHub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sally\Downloads\LAB_2_JFME-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55043317-14D3-43C9-88F0-43B8AE1B5AE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5959D808-1B92-40BB-A330-B741C98743B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{43A1268E-D998-4EED-B449-93D84121C54D}"/>
   </bookViews>

</xml_diff>